<commit_message>
Add file Database + update ERD
</commit_message>
<xml_diff>
--- a/Documents/SWP391-Backlog_Group3.xlsx
+++ b/Documents/SWP391-Backlog_Group3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\SWP391\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E632D8E-8AC2-4A65-8661-98BC73542BB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA43AFF5-F823-470E-B7AD-2F77106DB595}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DF743DC6-3E10-FC40-A74C-7ADFA9B03788}"/>
   </bookViews>
@@ -363,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -386,13 +386,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,6 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -822,8 +834,8 @@
   </sheetPr>
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1553,11 +1565,11 @@
       <c r="D34" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>38</v>
+      <c r="E34" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>46</v>
@@ -1580,10 +1592,10 @@
         <v>46</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>46</v>

</xml_diff>